<commit_message>
Updated xlsx and system pic.
</commit_message>
<xml_diff>
--- a/convacc/Table-conv-input-pp.xlsx
+++ b/convacc/Table-conv-input-pp.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="101">
   <si>
     <t>Cell</t>
   </si>
@@ -140,6 +140,36 @@
     <t>0x00_C600_0FFF</t>
   </si>
   <si>
+    <t>axi_bram_ctrl_4</t>
+  </si>
+  <si>
+    <t>0x00_C800_0000</t>
+  </si>
+  <si>
+    <t>0x00_C800_0FFF</t>
+  </si>
+  <si>
+    <t>axi_bram_ctrl_5</t>
+  </si>
+  <si>
+    <t>0x00_CA00_0000</t>
+  </si>
+  <si>
+    <t>0x00_CA00_7FFF</t>
+  </si>
+  <si>
+    <t>axi_bram_ctrl_6</t>
+  </si>
+  <si>
+    <t>0x00_CC00_0000</t>
+  </si>
+  <si>
+    <t>8K</t>
+  </si>
+  <si>
+    <t>0x00_CC00_1FFF</t>
+  </si>
+  <si>
     <t>M_AXI_SDA (22 address bits : 4M)</t>
   </si>
   <si>
@@ -245,55 +275,46 @@
     <t>0x0000_0000_C600_0FFF</t>
   </si>
   <si>
+    <t>0x0000_0000_C800_0000</t>
+  </si>
+  <si>
+    <t>0x0000_0000_C800_0FFF</t>
+  </si>
+  <si>
+    <t>0x0000_0000_CA00_0000</t>
+  </si>
+  <si>
+    <t>0x0000_0000_CA00_7FFF</t>
+  </si>
+  <si>
+    <t>0x0000_0000_CC00_0000</t>
+  </si>
+  <si>
+    <t>0x0000_0000_CC00_1FFF</t>
+  </si>
+  <si>
     <t>Data_m_axi_conv_weight_port (32 address bits : 4G)</t>
   </si>
   <si>
-    <t>0xC000_0000</t>
-  </si>
-  <si>
-    <t>8K</t>
-  </si>
-  <si>
-    <t>0xC000_1FFF</t>
-  </si>
-  <si>
-    <t>0xC200_0000</t>
-  </si>
-  <si>
-    <t>0xC200_1FFF</t>
-  </si>
-  <si>
-    <t>0xC400_0000</t>
-  </si>
-  <si>
-    <t>0xC400_1FFF</t>
-  </si>
-  <si>
-    <t>0xC600_0000</t>
-  </si>
-  <si>
-    <t>0xC600_1FFF</t>
-  </si>
-  <si>
-    <t>0x0000_0000</t>
-  </si>
-  <si>
-    <t>0x7FFF_FFFF</t>
-  </si>
-  <si>
-    <t>0x8000_0000</t>
-  </si>
-  <si>
-    <t>1G</t>
-  </si>
-  <si>
-    <t>0xBFFF_FFFF</t>
-  </si>
-  <si>
-    <t>Unmapped Slaves (2)</t>
+    <t>axi_bram_ctrl_7</t>
+  </si>
+  <si>
+    <t>0xCA00_0000</t>
+  </si>
+  <si>
+    <t>0xCA00_7FFF</t>
   </si>
   <si>
     <t>Data_m_axi_conv_bias_port (32 address bits : 4G)</t>
+  </si>
+  <si>
+    <t>axi_bram_ctrl_8</t>
+  </si>
+  <si>
+    <t>0xCC00_0000</t>
+  </si>
+  <si>
+    <t>0xCC00_1FFF</t>
   </si>
 </sst>
 </file>
@@ -339,7 +360,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
       <alignment horizontal="general" vertical="top"/>
@@ -352,9 +373,6 @@
     </xf>
     <xf numFmtId="18" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true">
       <alignment horizontal="general" vertical="top" indent="2"/>
-    </xf>
-    <xf numFmtId="18" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true">
-      <alignment horizontal="general" vertical="top" indent="3"/>
     </xf>
   </cellXfs>
 </styleSheet>
@@ -369,7 +387,7 @@
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" outlineLevelRow="3"/>
+  <sheetFormatPr defaultRowHeight="15.0" outlineLevelRow="2"/>
   <cols>
     <col min="1" max="1" width="11.71875" customWidth="true"/>
     <col min="2" max="2" width="11.71875" customWidth="true"/>
@@ -599,244 +617,244 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" outlineLevel="1">
-      <c r="A12" t="s" s="3">
+    <row r="12" outlineLevel="2">
+      <c r="A12" t="s" s="4">
         <v>42</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s" s="2">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="D12" t="s" s="2">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E12" t="s" s="2">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="F12" t="s" s="2">
-        <v>7</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" outlineLevel="2">
       <c r="A13" t="s" s="4">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s" s="2">
         <v>27</v>
       </c>
       <c r="C13" t="s" s="2">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="D13" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E13" t="s" s="2">
+        <v>30</v>
+      </c>
+      <c r="F13" t="s" s="2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" outlineLevel="2">
+      <c r="A14" t="s" s="4">
+        <v>48</v>
+      </c>
+      <c r="B14" t="s" s="2">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s" s="2">
+        <v>28</v>
+      </c>
+      <c r="D14" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="E14" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="F14" t="s" s="2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" outlineLevel="1">
+      <c r="A15" t="s" s="3">
+        <v>52</v>
+      </c>
+      <c r="B15" t="s" s="2">
+        <v>7</v>
+      </c>
+      <c r="C15" t="s" s="2">
+        <v>7</v>
+      </c>
+      <c r="D15" t="s" s="2">
+        <v>7</v>
+      </c>
+      <c r="E15" t="s" s="2">
+        <v>7</v>
+      </c>
+      <c r="F15" t="s" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" outlineLevel="2">
+      <c r="A16" t="s" s="4">
+        <v>53</v>
+      </c>
+      <c r="B16" t="s" s="2">
+        <v>27</v>
+      </c>
+      <c r="C16" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="D16" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="E16" t="s" s="2">
         <v>40</v>
       </c>
-      <c r="F13" t="s" s="2">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" outlineLevel="1">
-      <c r="A14" t="s" s="3">
-        <v>47</v>
-      </c>
-      <c r="B14" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="C14" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="D14" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="E14" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="F14" t="s" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" outlineLevel="2">
-      <c r="A15" t="s" s="4">
-        <v>48</v>
-      </c>
-      <c r="B15" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="C15" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="D15" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="E15" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="F15" t="s" s="2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" outlineLevel="1">
-      <c r="A16" t="s" s="3">
-        <v>51</v>
-      </c>
-      <c r="B16" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="C16" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="D16" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="E16" t="s" s="2">
-        <v>7</v>
-      </c>
       <c r="F16" t="s" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" outlineLevel="2">
-      <c r="A17" t="s" s="4">
-        <v>52</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" outlineLevel="1">
+      <c r="A17" t="s" s="3">
+        <v>57</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="C17" t="s" s="2">
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="D17" t="s" s="2">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="E17" t="s" s="2">
-        <v>54</v>
+        <v>7</v>
       </c>
       <c r="F17" t="s" s="2">
-        <v>55</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" outlineLevel="2">
       <c r="A18" t="s" s="4">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="C18" t="s" s="2">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="D18" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E18" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="F18" t="s" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" outlineLevel="1">
+      <c r="A19" t="s" s="3">
+        <v>61</v>
+      </c>
+      <c r="B19" t="s" s="2">
+        <v>7</v>
+      </c>
+      <c r="C19" t="s" s="2">
+        <v>7</v>
+      </c>
+      <c r="D19" t="s" s="2">
+        <v>7</v>
+      </c>
+      <c r="E19" t="s" s="2">
+        <v>7</v>
+      </c>
+      <c r="F19" t="s" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" outlineLevel="2">
+      <c r="A20" t="s" s="4">
+        <v>62</v>
+      </c>
+      <c r="B20" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="C20" t="s" s="2">
         <v>54</v>
       </c>
-      <c r="F18" t="s" s="2">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="B19" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="C19" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="D19" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="E19" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="F19" t="s" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" outlineLevel="1">
-      <c r="A20" t="s" s="3">
-        <v>60</v>
-      </c>
-      <c r="B20" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="C20" t="s" s="2">
-        <v>7</v>
-      </c>
       <c r="D20" t="s" s="2">
-        <v>7</v>
+        <v>55</v>
       </c>
       <c r="E20" t="s" s="2">
-        <v>7</v>
+        <v>64</v>
       </c>
       <c r="F20" t="s" s="2">
-        <v>7</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" outlineLevel="2">
       <c r="A21" t="s" s="4">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>9</v>
+        <v>67</v>
       </c>
       <c r="C21" t="s" s="2">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="D21" t="s" s="2">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="E21" t="s" s="2">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="F21" t="s" s="2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="2">
         <v>62</v>
       </c>
-    </row>
-    <row r="22" outlineLevel="2">
-      <c r="A22" t="s" s="4">
-        <v>6</v>
-      </c>
       <c r="B22" t="s" s="2">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C22" t="s" s="2">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D22" t="s" s="2">
-        <v>63</v>
+        <v>7</v>
       </c>
       <c r="E22" t="s" s="2">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F22" t="s" s="2">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" outlineLevel="2">
-      <c r="A23" t="s" s="4">
-        <v>6</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" outlineLevel="1">
+      <c r="A23" t="s" s="3">
+        <v>70</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C23" t="s" s="2">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D23" t="s" s="2">
-        <v>65</v>
+        <v>7</v>
       </c>
       <c r="E23" t="s" s="2">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F23" t="s" s="2">
-        <v>66</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" outlineLevel="2">
@@ -844,84 +862,84 @@
         <v>6</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C24" t="s" s="2">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="D24" t="s" s="2">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="E24" t="s" s="2">
         <v>12</v>
       </c>
       <c r="F24" t="s" s="2">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" outlineLevel="2">
       <c r="A25" t="s" s="4">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C25" t="s" s="2">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="D25" t="s" s="2">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="E25" t="s" s="2">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="F25" t="s" s="2">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" outlineLevel="2">
       <c r="A26" t="s" s="4">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C26" t="s" s="2">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D26" t="s" s="2">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E26" t="s" s="2">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="F26" t="s" s="2">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" outlineLevel="2">
       <c r="A27" t="s" s="4">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C27" t="s" s="2">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D27" t="s" s="2">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E27" t="s" s="2">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="F27" t="s" s="2">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" outlineLevel="2">
       <c r="A28" t="s" s="4">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="B28" t="s" s="2">
         <v>27</v>
@@ -930,58 +948,58 @@
         <v>28</v>
       </c>
       <c r="D28" t="s" s="2">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="E28" t="s" s="2">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="F28" t="s" s="2">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="s" s="2">
-        <v>56</v>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" outlineLevel="2">
+      <c r="A29" t="s" s="4">
+        <v>32</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="C29" t="s" s="2">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="D29" t="s" s="2">
-        <v>7</v>
+        <v>81</v>
       </c>
       <c r="E29" t="s" s="2">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="F29" t="s" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" outlineLevel="1">
-      <c r="A30" t="s" s="3">
-        <v>77</v>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" outlineLevel="2">
+      <c r="A30" t="s" s="4">
+        <v>35</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="C30" t="s" s="2">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="D30" t="s" s="2">
-        <v>7</v>
+        <v>83</v>
       </c>
       <c r="E30" t="s" s="2">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="F30" t="s" s="2">
-        <v>7</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" outlineLevel="2">
       <c r="A31" t="s" s="4">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="B31" t="s" s="2">
         <v>27</v>
@@ -990,18 +1008,18 @@
         <v>28</v>
       </c>
       <c r="D31" t="s" s="2">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="E31" t="s" s="2">
-        <v>79</v>
+        <v>40</v>
       </c>
       <c r="F31" t="s" s="2">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" outlineLevel="2">
       <c r="A32" t="s" s="4">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="B32" t="s" s="2">
         <v>27</v>
@@ -1010,18 +1028,18 @@
         <v>28</v>
       </c>
       <c r="D32" t="s" s="2">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E32" t="s" s="2">
-        <v>79</v>
+        <v>40</v>
       </c>
       <c r="F32" t="s" s="2">
-        <v>82</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" outlineLevel="2">
       <c r="A33" t="s" s="4">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="B33" t="s" s="2">
         <v>27</v>
@@ -1030,18 +1048,18 @@
         <v>28</v>
       </c>
       <c r="D33" t="s" s="2">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="E33" t="s" s="2">
-        <v>79</v>
+        <v>30</v>
       </c>
       <c r="F33" t="s" s="2">
-        <v>84</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" outlineLevel="2">
       <c r="A34" t="s" s="4">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B34" t="s" s="2">
         <v>27</v>
@@ -1050,84 +1068,84 @@
         <v>28</v>
       </c>
       <c r="D34" t="s" s="2">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="E34" t="s" s="2">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="F34" t="s" s="2">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="35" outlineLevel="2">
-      <c r="A35" t="s" s="4">
-        <v>6</v>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="2">
+        <v>66</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C35" t="s" s="2">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D35" t="s" s="2">
-        <v>87</v>
+        <v>7</v>
       </c>
       <c r="E35" t="s" s="2">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F35" t="s" s="2">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="36" outlineLevel="2">
-      <c r="A36" t="s" s="4">
-        <v>6</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" outlineLevel="1">
+      <c r="A36" t="s" s="3">
+        <v>93</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C36" t="s" s="2">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D36" t="s" s="2">
-        <v>89</v>
+        <v>7</v>
       </c>
       <c r="E36" t="s" s="2">
-        <v>90</v>
+        <v>7</v>
       </c>
       <c r="F36" t="s" s="2">
-        <v>91</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" outlineLevel="2">
       <c r="A37" t="s" s="4">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="C37" t="s" s="2">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="D37" t="s" s="2">
-        <v>7</v>
+        <v>95</v>
       </c>
       <c r="E37" t="s" s="2">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="F37" t="s" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" outlineLevel="3">
-      <c r="A38" t="s" s="5">
-        <v>6</v>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" outlineLevel="1">
+      <c r="A38" t="s" s="3">
+        <v>97</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C38" t="s" s="2">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D38" t="s" s="2">
         <v>7</v>
@@ -1139,240 +1157,38 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" outlineLevel="3">
-      <c r="A39" t="s" s="5">
-        <v>6</v>
+    <row r="39" outlineLevel="2">
+      <c r="A39" t="s" s="4">
+        <v>98</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C39" t="s" s="2">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D39" t="s" s="2">
-        <v>7</v>
+        <v>99</v>
       </c>
       <c r="E39" t="s" s="2">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="F39" t="s" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" outlineLevel="1">
-      <c r="A40" t="s" s="3">
-        <v>93</v>
-      </c>
-      <c r="B40" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="C40" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="D40" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="E40" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="F40" t="s" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" outlineLevel="2">
-      <c r="A41" t="s" s="4">
-        <v>26</v>
-      </c>
-      <c r="B41" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="C41" t="s" s="2">
-        <v>28</v>
-      </c>
-      <c r="D41" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="E41" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="F41" t="s" s="2">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="42" outlineLevel="2">
-      <c r="A42" t="s" s="4">
-        <v>32</v>
-      </c>
-      <c r="B42" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="C42" t="s" s="2">
-        <v>28</v>
-      </c>
-      <c r="D42" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="E42" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="F42" t="s" s="2">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="43" outlineLevel="2">
-      <c r="A43" t="s" s="4">
-        <v>35</v>
-      </c>
-      <c r="B43" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="C43" t="s" s="2">
-        <v>28</v>
-      </c>
-      <c r="D43" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="E43" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="F43" t="s" s="2">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="44" outlineLevel="2">
-      <c r="A44" t="s" s="4">
-        <v>38</v>
-      </c>
-      <c r="B44" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="C44" t="s" s="2">
-        <v>28</v>
-      </c>
-      <c r="D44" t="s" s="2">
-        <v>85</v>
-      </c>
-      <c r="E44" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="F44" t="s" s="2">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="45" outlineLevel="2">
-      <c r="A45" t="s" s="4">
-        <v>6</v>
-      </c>
-      <c r="B45" t="s" s="2">
-        <v>9</v>
-      </c>
-      <c r="C45" t="s" s="2">
-        <v>10</v>
-      </c>
-      <c r="D45" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="E45" t="s" s="2">
-        <v>12</v>
-      </c>
-      <c r="F45" t="s" s="2">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="46" outlineLevel="2">
-      <c r="A46" t="s" s="4">
-        <v>6</v>
-      </c>
-      <c r="B46" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="C46" t="s" s="2">
-        <v>15</v>
-      </c>
-      <c r="D46" t="s" s="2">
-        <v>89</v>
-      </c>
-      <c r="E46" t="s" s="2">
-        <v>90</v>
-      </c>
-      <c r="F46" t="s" s="2">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="47" outlineLevel="2">
-      <c r="A47" t="s" s="4">
-        <v>92</v>
-      </c>
-      <c r="B47" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="C47" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="D47" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="E47" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="F47" t="s" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="48" outlineLevel="3">
-      <c r="A48" t="s" s="5">
-        <v>6</v>
-      </c>
-      <c r="B48" t="s" s="2">
-        <v>18</v>
-      </c>
-      <c r="C48" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="D48" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="E48" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="F48" t="s" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="49" outlineLevel="3">
-      <c r="A49" t="s" s="5">
-        <v>6</v>
-      </c>
-      <c r="B49" t="s" s="2">
-        <v>22</v>
-      </c>
-      <c r="C49" t="s" s="2">
-        <v>23</v>
-      </c>
-      <c r="D49" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="E49" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="F49" t="s" s="2">
-        <v>7</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="A14:F14"/>
-    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="A17:F17"/>
     <mergeCell ref="A19:F19"/>
-    <mergeCell ref="A20:F20"/>
-    <mergeCell ref="A29:F29"/>
-    <mergeCell ref="A30:F30"/>
-    <mergeCell ref="A37:F37"/>
-    <mergeCell ref="A40:F40"/>
-    <mergeCell ref="A47:F47"/>
+    <mergeCell ref="A22:F22"/>
+    <mergeCell ref="A23:F23"/>
+    <mergeCell ref="A35:F35"/>
+    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="A38:F38"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>